<commit_message>
User Stories - Acceptance Criteria
1.1
</commit_message>
<xml_diff>
--- a/User Stories - Acceptance Criteria.xlsx
+++ b/User Stories - Acceptance Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Y2\S2\Software Engineering\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F14D5-E5C0-45B3-B6B2-33AC731BABD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897732EC-2A66-4D3C-AD11-CE96E414E2BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{ADFB4776-4ACB-4BCD-AA74-3846904141C1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>User Story</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Program must be able to read from database</t>
-  </si>
-  <si>
-    <t>UI must be capable of testing implemented functions</t>
   </si>
   <si>
     <t>User can only log in when username and password are both correct</t>
@@ -501,7 +498,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,19 +607,17 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -633,10 +628,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -646,7 +641,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -657,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -665,10 +660,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -679,7 +674,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>

</xml_diff>